<commit_message>
update metab reactor costing
</commit_message>
<xml_diff>
--- a/exposan/metab_mock/data/HDPE_pipe_chart.xlsx
+++ b/exposan/metab_mock/data/HDPE_pipe_chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\metab_mock\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C26CD0-7FB1-4B90-A688-B9862996AFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6EE4B8-7E26-4CFF-9658-9E5DBB7852C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="15552" windowHeight="9054" xr2:uid="{1A6FEF34-8B04-4585-AC04-C20E8D75E96E}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{1A6FEF34-8B04-4585-AC04-C20E8D75E96E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>OD</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>Size</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>USD/ft</t>
+  </si>
+  <si>
+    <t>USD/lbs</t>
+  </si>
+  <si>
+    <t>USD/kg</t>
   </si>
 </sst>
 </file>
@@ -98,8 +110,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -115,6 +130,1150 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Price [USD/kg]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.35297078338471366"/>
+          <c:y val="7.7380952380952384E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.8214029331152294E-2"/>
+          <c:y val="6.0059523809523827E-2"/>
+          <c:w val="0.83802854391203563"/>
+          <c:h val="0.74111126734158228"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1:$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Price</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>USD/kg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:backward val="1"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.7265727463231201E-2"/>
+                  <c:y val="-0.29561679790026246"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1.34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.917</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8260000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.633</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3490000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9630000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.6790000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.292999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.301</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.914999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.532</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.146000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17.760000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.373999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.988</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.605</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24.219000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25.832999999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27.446999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>29.061</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>33.905999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$3:$H$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>10.311998401284663</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.4100237724086284</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5794550144403541</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8050078819635722</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1250585874365058</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.6385502325889023</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.7840821146309276</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.6471543366527257</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.6486693961013987</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.9350387907123605</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.747085132096621</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.5899954523446862</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.453912849416787</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.3352728930160596</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.2300397649089776</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.1366842041153018</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.0529708208782291</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.9764590329167175</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.9069170031700762</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8428482686267582</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.7837633433153846</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.6308142727445811</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BC69-400A-BD4E-D1004C4417E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="159937472"/>
+        <c:axId val="159938720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="159937472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ID [inch]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="159938720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="159938720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="159937472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>470535</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>369570</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A01AF18-CA9D-D07F-E776-64A379E8BD6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,15 +1573,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA2F41B3-AECC-4C51-B20F-2AD0316B9A67}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -438,8 +1597,13 @@
       <c r="E1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -455,8 +1619,17 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>1.25</v>
       </c>
@@ -472,8 +1645,19 @@
       <c r="E3">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F3">
+        <v>1.45</v>
+      </c>
+      <c r="G3">
+        <f>F3/E3</f>
+        <v>4.67741935483871</v>
+      </c>
+      <c r="H3">
+        <f>G3/0.45359</f>
+        <v>10.311998401284663</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>1.5</v>
       </c>
@@ -489,8 +1673,19 @@
       <c r="E4">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F4">
+        <v>1.75</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G11" si="0">F4/E4</f>
+        <v>4.2682926829268295</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H24" si="1">G4/0.45359</f>
+        <v>9.4100237724086284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>2</v>
       </c>
@@ -506,8 +1701,19 @@
       <c r="E5">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F5">
+        <v>1.91</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>2.984375</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>6.5794550144403541</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>3</v>
       </c>
@@ -523,8 +1729,19 @@
       <c r="E6">
         <v>1.39</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F6">
+        <v>3.66</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>2.6330935251798566</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>5.8050078819635722</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>4</v>
       </c>
@@ -540,8 +1757,19 @@
       <c r="E7">
         <v>2.31</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F7">
+        <v>5.37</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>2.3246753246753245</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>5.1250585874365058</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>6</v>
       </c>
@@ -557,8 +1785,19 @@
       <c r="E8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F8">
+        <v>10.52</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>2.1040000000000001</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>4.6385502325889023</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>8</v>
       </c>
@@ -574,8 +1813,19 @@
       <c r="E9">
         <v>8.4700000000000006</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F9">
+        <v>18.38</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>2.1700118063754426</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>4.7840821146309276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>10</v>
       </c>
@@ -591,8 +1841,19 @@
       <c r="E10">
         <v>13.16</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F10">
+        <v>27.74</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>2.1079027355623099</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>4.6471543366527257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>12</v>
       </c>
@@ -608,8 +1869,19 @@
       <c r="E11">
         <v>18.510000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F11">
+        <v>39.03</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>2.1085899513776334</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>4.6486693961013987</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>14</v>
       </c>
@@ -625,8 +1897,20 @@
       <c r="E12">
         <v>22.32</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F12">
+        <f>0.7592*D12^1.6332</f>
+        <v>39.838839550168181</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:G24" si="2">F12/E12</f>
+        <v>1.7848942450792196</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>3.9350387907123605</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>16</v>
       </c>
@@ -642,8 +1926,20 @@
       <c r="E13">
         <v>29.15</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F13">
+        <f t="shared" ref="F13:F24" si="3">0.7592*D13^1.6332</f>
+        <v>49.544516058723637</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>1.6996403450677062</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>3.747085132096621</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>18</v>
       </c>
@@ -659,8 +1955,20 @@
       <c r="E14">
         <v>36.89</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>60.071160913378776</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>1.6283860372290262</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>3.5899954523446862</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>20</v>
       </c>
@@ -676,8 +1984,20 @@
       <c r="E15">
         <v>45.54</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>71.345711399371368</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>1.5666603293669603</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>3.453912849416787</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>22</v>
       </c>
@@ -693,8 +2013,20 @@
       <c r="E16">
         <v>55.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>83.357838378027807</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>1.5128464315431545</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>3.3352728930160596</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>24</v>
       </c>
@@ -710,8 +2042,20 @@
       <c r="E17">
         <v>65.58</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>96.08215887016884</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>1.4651137369650631</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>3.2300397649089776</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>26</v>
       </c>
@@ -727,8 +2071,20 @@
       <c r="E18">
         <v>76.959999999999994</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>109.49627054361301</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>1.4227685881446597</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>3.1366842041153018</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>28</v>
       </c>
@@ -744,8 +2100,20 @@
       <c r="E19">
         <v>89.26</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>123.60698331215885</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>1.3847970346421559</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>3.0529708208782291</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>30</v>
       </c>
@@ -761,8 +2129,20 @@
       <c r="E20">
         <v>102.47</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>138.34393264433891</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>1.3500920527406939</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>2.9764590329167175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>32</v>
       </c>
@@ -778,8 +2158,20 @@
       <c r="E21">
         <v>116.58</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F21">
+        <f t="shared" si="3"/>
+        <v>153.71638220268952</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>1.3185484834679149</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>2.9069170031700762</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>34</v>
       </c>
@@ -795,8 +2187,20 @@
       <c r="E22">
         <v>131.61000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F22">
+        <f t="shared" si="3"/>
+        <v>169.7094559509614</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>1.2894875461664113</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>2.8428482686267582</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>36</v>
       </c>
@@ -812,8 +2216,20 @@
       <c r="E23">
         <v>147.55000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F23">
+        <f t="shared" si="3"/>
+        <v>186.30949855767247</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>1.2626872148944253</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>2.7837633433153846</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>42</v>
       </c>
@@ -829,8 +2245,24 @@
       <c r="E24">
         <v>200.84</v>
       </c>
+      <c r="F24">
+        <f t="shared" si="3"/>
+        <v>239.66459047346123</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>1.1933110459742144</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>2.6308142727445811</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>